<commit_message>
updated times effort Obed
</commit_message>
<xml_diff>
--- a/Tiempos.xlsx
+++ b/Tiempos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://argoscorp-my.sharepoint.com/personal/orios_argos_com_co/Documents/Documentos/Projekte/0. Bitacora/Master/EC1209/metodos-estadisticos-avanzados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orios\OneDrive - Cementos Argos S.A\Documentos\Projekte\0. Bitacora\Master\EC1209\metodos-estadisticos-avanzados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F217FF2-1E6C-4CF6-A00D-7EC0EB6585AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{0F217FF2-1E6C-4CF6-A00D-7EC0EB6585AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0BA6F8A7-DB82-4119-BC8F-6905DF09DE8F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4FA5149C-B21D-42BA-92EC-77E2EB93F583}"/>
   </bookViews>
@@ -408,7 +408,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,7 +445,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -461,7 +461,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -470,6 +470,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101005AFBDC1B44A49B40B242C2635A71736C" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="aec19bb90c2f603cbb423caecdc9711c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ba47b03c-b346-4b4c-97b6-67031c6cde0c" xmlns:ns4="e1c1edfb-439f-4bef-83ea-377a08ce178f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b33c2bcb400664243110d4af64e868f9" ns3:_="" ns4:_="">
     <xsd:import namespace="ba47b03c-b346-4b4c-97b6-67031c6cde0c"/>
@@ -692,22 +707,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05EEA3F0-75D3-48F1-A105-F7B1DEEFC415}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25B17C83-9C49-4DB0-A94F-F5B88762BC6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B54E9A9B-EAE5-479A-AE07-B02D0F1F6DB7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -724,21 +741,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25B17C83-9C49-4DB0-A94F-F5B88762BC6D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05EEA3F0-75D3-48F1-A105-F7B1DEEFC415}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>